<commit_message>
Changed parameters and excel
</commit_message>
<xml_diff>
--- a/data/LCOEBENCE(1).xlsx
+++ b/data/LCOEBENCE(1).xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanko\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f40ad5fc536dd58c/Desktop/Oxford/OPV/OPVSBSP_Code/OPV_SBSP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED5EEA6-4DE4-4122-8881-471E05AA7EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:1_{DED5EEA6-4DE4-4122-8881-471E05AA7EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06F08B93-0266-422E-8F91-6A0A4078739C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5EE87DF2-9FC5-4DDF-A454-2AABC6FB7A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Information" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="130">
   <si>
     <t>LCOE</t>
   </si>
@@ -80,9 +81,6 @@
     <t>Mean</t>
   </si>
   <si>
-    <t>Most Likely</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -161,9 +159,6 @@
     <t>Emission Cost</t>
   </si>
   <si>
-    <t>Yearly?</t>
-  </si>
-  <si>
     <t>Regulations and market mechanisms to cause a wide but evenly spread range of costs.</t>
   </si>
   <si>
@@ -297,13 +292,350 @@
   </si>
   <si>
     <t>Energy Genrated</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>Uniform</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>log-normal</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Represents the average number of events in a fixed interval of time or space.</t>
+  </si>
+  <si>
+    <r>
+      <t>Shape</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Also known as the k parameter, it influences the skewness of the distribution.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Scale</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Often referred to as theta (θ), it stretches or compresses the distribution</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Shape</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Two parameters, α (alpha) and β (beta), defining the shape of the distribution.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Scale</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Typically, this distribution is defined on the interval [0, 1], and scale parameters modify its concentration.</t>
+    </r>
+  </si>
+  <si>
+    <t>Scale for exponential</t>
+  </si>
+  <si>
+    <r>
+      <t>Scale (θ = 1/λ):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This parameter tells you the average time between events. For example, if λ\lambdaλ (rate) is 2 events per hour, the scale (θ) would be 0.5 hours per event. This means, on average, an event occurs every 0.5 hours.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A Higher Scale Value:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Indicates that events happen less frequently (longer expected time until the next event).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A Lower Scale Value:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Indicates that events happen more frequently (shorter expected time until the next event).</t>
+    </r>
+  </si>
+  <si>
+    <t>The Gamma distribution is commonly used to model waiting times for a specified number of events, especially when these events follow a Poisson process.</t>
+  </si>
+  <si>
+    <t>Parameters:</t>
+  </si>
+  <si>
+    <r>
+      <t>Shape (k)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: This parameter is also known as the shape parameter or sometimes the "order" of the distribution. It affects the form of the probability distribution.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Scale (θ)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: This parameter stretches or compresses the distribution along the horizontal axis.</t>
+    </r>
+  </si>
+  <si>
+    <t>Probability Density Function (PDF):</t>
+  </si>
+  <si>
+    <t>The PDF of the Gamma distribution is given by: f(x;k,θ)=xk−1e−xθθkΓ(k)f(x; k, \theta) = \frac{x^{k-1} e^{-\frac{x}{\theta}}}{\theta^k \Gamma(k)}f(x;k,θ)=θkΓ(k)xk−1e−θx​​ where:</t>
+  </si>
+  <si>
+    <t>x≥0x \geq 0x≥0</t>
+  </si>
+  <si>
+    <t>Γ(k)\Gamma(k)Γ(k) is the gamma function, which generalizes the factorial function with Γ(n)=(n−1)!\Gamma(n) = (n-1)!Γ(n)=(n−1)! for integer nnn.</t>
+  </si>
+  <si>
+    <t>Calculating Shape and Scale:</t>
+  </si>
+  <si>
+    <r>
+      <t>Shape (k)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: This is often derived from the data or expected values. For instance, if you know the average number of events and the variance, kkk can be estimated as μ2σ2\frac{\mu^2}{\sigma^2}σ2μ2​, where μ\muμ is the mean and σ2\sigma^2σ2 is the variance.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Scale (θ)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Once you have kkk, θ\thetaθ can be calculated as θ=σ2μ\theta = \frac{\sigma^2}{\mu}θ=μσ2​.</t>
+    </r>
+  </si>
+  <si>
+    <t>The Beta distribution is useful for modelling variables that are constrained to an interval, such as probabilities. It's often used in Bayesian statistics.</t>
+  </si>
+  <si>
+    <r>
+      <t>Shape (α, β)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: These two parameters define the shape of the distribution. They control the height and skewness of the distribution's curve.</t>
+    </r>
+  </si>
+  <si>
+    <t>The PDF of the Beta distribution is: f(x;α,β)=xα−1(1−x)β−1B(α,β)f(x; \alpha, \beta) = \frac{x^{\alpha-1} (1-x)^{\beta-1}}{B(\alpha, \beta)}f(x;α,β)=B(α,β)xα−1(1−x)β−1​ where:</t>
+  </si>
+  <si>
+    <t>0≤x≤10 \leq x \leq 10≤x≤1</t>
+  </si>
+  <si>
+    <t>B(α,β)B(\alpha, \beta)B(α,β) is the beta function, which serves as a normalization constant to ensure the total probability is 1.</t>
+  </si>
+  <si>
+    <t>Calculating Shape Parameters:</t>
+  </si>
+  <si>
+    <r>
+      <t>Shape (α and β)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: These are typically estimated based on prior knowledge or inferred statistically from data. For instance, if you know the mean μ\muμ and variance σ2\sigma^2σ2 of the data, α\alphaα and β\betaβ can be derived using: α=μ((1−μ)σ2−1μ)\alpha = \mu \left( \frac{(1 - \mu)}{\sigma^2} - \frac{1}{\mu} \right)α=μ(σ2(1−μ)​−μ1​) β=(1−μ)(μσ2−11−μ)\beta = (1 - \mu) \left( \frac{\mu}{\sigma^2} - \frac{1}{1 - \mu} \right)β=(1−μ)(σ2μ​−1−μ1​)</t>
+    </r>
+  </si>
+  <si>
+    <t>In practical terms, for Monte Carlo simulation:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gamma distribution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, if you're modelling time until a number of events occur, you'd estimate kkk and θ\thetaθ based on historical event frequency and spread.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Beta distribution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, when simulating probabilities (like component reliability or achieving a target within constraints), you'd set α\alphaα and β\betaβ to shape the distribution according to known or expected performance.</t>
+    </r>
+  </si>
+  <si>
+    <t>Shape is alpha</t>
+  </si>
+  <si>
+    <t>scale is beta</t>
+  </si>
+  <si>
+    <t>Material Repairs Cost</t>
+  </si>
+  <si>
+    <t>Bernoulli</t>
+  </si>
+  <si>
+    <t>£/panel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,8 +651,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -417,6 +757,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -458,7 +804,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -514,16 +860,35 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="21">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -569,7 +934,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -592,7 +957,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -615,7 +980,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -638,7 +1003,53 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -922,25 +1333,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{909B92F7-FD86-4123-9D2B-E5C0FFDF9F53}" name="Table142" displayName="Table142" ref="B3:Q26" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="B3:Q26" xr:uid="{909B92F7-FD86-4123-9D2B-E5C0FFDF9F53}"/>
-  <tableColumns count="16">
-    <tableColumn id="2" xr3:uid="{AE1E91F8-E08D-4870-9EA0-9D766B95EB09}" name="Primary" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{117D9C5B-B5EB-4229-8E6B-F43AA68FDD63}" name="Secondary" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{E20BFF9A-E6DB-4DA8-B61C-78AD62869AB0}" name="Tertiary" dataDxfId="13"/>
-    <tableColumn id="15" xr3:uid="{AC0B1E94-75E6-4D82-93A4-33F5480F0B94}" name="Quaternary" dataDxfId="12"/>
-    <tableColumn id="16" xr3:uid="{C1AC552C-A369-4000-876A-E0CEC4E0E60C}" name="Quintenary" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{DCB5AB7C-8BE9-4156-8808-C7844619DC70}" name="Relationships" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{E494D826-7428-44F0-8A41-82212B791038}" name="Multiplied" dataDxfId="9"/>
-    <tableColumn id="1" xr3:uid="{9562A130-14D3-4A9B-9FC6-6563E1EBD9FD}" name="Units" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{0E83D34C-CD9E-4572-948B-530B8A0AC574}" name="Distribution" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{F85CB51D-AECB-435B-8E6E-86A6A19C6EE6}" name="Time for determination (Year)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{796FC7BB-E419-482C-AED0-2D0EC27F353E}" name="Lower Limit" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{E8F799E3-4165-4BB4-B4E3-E0AC59BF7E53}" name="Upper Limit" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{A05EEDE8-7B8A-4237-951E-78D9F4E5CDCF}" name="SD" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{0CF3F9E6-935B-4AB5-8103-35660404BC57}" name="Mean" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{ED5B0C21-BE1E-4570-BC5D-006BB2D1AC04}" name="Most Likely" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{3CF19983-7617-4E79-BA6C-E9BD88BF77AC}" name="Comments" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{909B92F7-FD86-4123-9D2B-E5C0FFDF9F53}" name="Table142" displayName="Table142" ref="B3:S27" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+  <autoFilter ref="B3:S27" xr:uid="{909B92F7-FD86-4123-9D2B-E5C0FFDF9F53}"/>
+  <tableColumns count="18">
+    <tableColumn id="2" xr3:uid="{AE1E91F8-E08D-4870-9EA0-9D766B95EB09}" name="Primary" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{117D9C5B-B5EB-4229-8E6B-F43AA68FDD63}" name="Secondary" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{E20BFF9A-E6DB-4DA8-B61C-78AD62869AB0}" name="Tertiary" dataDxfId="15"/>
+    <tableColumn id="15" xr3:uid="{AC0B1E94-75E6-4D82-93A4-33F5480F0B94}" name="Quaternary" dataDxfId="14"/>
+    <tableColumn id="16" xr3:uid="{C1AC552C-A369-4000-876A-E0CEC4E0E60C}" name="Quintenary" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{DCB5AB7C-8BE9-4156-8808-C7844619DC70}" name="Relationships" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{E494D826-7428-44F0-8A41-82212B791038}" name="Multiplied" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{9562A130-14D3-4A9B-9FC6-6563E1EBD9FD}" name="Units" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{0E83D34C-CD9E-4572-948B-530B8A0AC574}" name="Distribution" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{F85CB51D-AECB-435B-8E6E-86A6A19C6EE6}" name="Time for determination (Year)" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{796FC7BB-E419-482C-AED0-2D0EC27F353E}" name="Lower Limit" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{E8F799E3-4165-4BB4-B4E3-E0AC59BF7E53}" name="Upper Limit" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{A05EEDE8-7B8A-4237-951E-78D9F4E5CDCF}" name="SD" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{0CF3F9E6-935B-4AB5-8103-35660404BC57}" name="Scale" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{ED5B0C21-BE1E-4570-BC5D-006BB2D1AC04}" name="Count" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{405E56AE-8602-44F1-B0E5-88A5D58A6492}" name="Shape" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{BD72848E-BEE6-471B-BAF7-23A9FDE1B8A8}" name="Mean" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{3CF19983-7617-4E79-BA6C-E9BD88BF77AC}" name="Comments" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1263,26 +1676,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14302A7-C5E8-40FF-86F2-64C01806B27A}">
-  <dimension ref="A2:Q26"/>
+  <dimension ref="A2:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="6" width="24.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.77734375" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.21875" style="1" customWidth="1"/>
-    <col min="12" max="16" width="8.88671875" style="1"/>
-    <col min="17" max="17" width="29.5546875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="1"/>
+    <col min="12" max="18" width="8.88671875" style="1"/>
+    <col min="19" max="19" width="29.5546875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1291,7 +1706,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:17" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1311,10 +1726,10 @@
         <v>6</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>7</v>
@@ -1335,181 +1750,206 @@
         <v>12</v>
       </c>
       <c r="O3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="H4" s="7">
+        <v>18</v>
+      </c>
       <c r="I4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24">
+        <v>20</v>
+      </c>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="D5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="5"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24">
+        <v>1000</v>
+      </c>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24">
+        <v>2</v>
+      </c>
+      <c r="R5" s="24"/>
+      <c r="S5" s="7"/>
+    </row>
+    <row r="6" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7">
         <v>1</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24">
+        <v>1000</v>
+      </c>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24">
         <v>2</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-    </row>
-    <row r="8" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="R7" s="24"/>
+      <c r="S7" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -1518,65 +1958,79 @@
         <v>2</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24">
+        <v>5000</v>
+      </c>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24">
+        <v>50000</v>
+      </c>
+      <c r="S8" s="7"/>
+    </row>
+    <row r="9" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24">
+        <v>2</v>
+      </c>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24">
+        <v>10</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1586,153 +2040,169 @@
         <v>3</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24">
+        <v>10</v>
+      </c>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24">
+        <v>100</v>
+      </c>
+      <c r="S10" s="7"/>
+    </row>
+    <row r="11" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I11" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-    </row>
-    <row r="12" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24">
+        <v>3</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="7" t="s">
-        <v>82</v>
-      </c>
+      <c r="G12" s="7"/>
       <c r="H12" s="7">
         <v>4</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-    </row>
-    <row r="13" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24">
+        <v>2000</v>
+      </c>
+      <c r="S12" s="7"/>
+    </row>
+    <row r="13" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F13" s="5"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="H13" s="7">
         <v>4</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24">
+        <v>-0.69889999999999997</v>
+      </c>
+      <c r="S13" s="7"/>
+    </row>
+    <row r="14" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="7"/>
@@ -1740,98 +2210,126 @@
         <v>4</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>47</v>
+        <v>128</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-    </row>
-    <row r="15" spans="1:17" ht="72" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="L14" s="24">
+        <v>365</v>
+      </c>
+      <c r="M14" s="24">
+        <v>366</v>
+      </c>
+      <c r="N14" s="24">
+        <v>0.24249999999999999</v>
+      </c>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24">
+        <v>365</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="F15" s="5"/>
-      <c r="G15" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="H15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7">
+        <v>4</v>
+      </c>
       <c r="I15" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K15" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24">
+        <v>24</v>
+      </c>
+      <c r="S15" s="7"/>
+    </row>
+    <row r="16" spans="1:19" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24">
+        <v>30</v>
+      </c>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24">
+        <v>3000</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1839,73 +2337,77 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="L17" s="24">
+        <v>0.06</v>
+      </c>
+      <c r="M17" s="24">
+        <v>0.08</v>
+      </c>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="7"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>62</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="7">
-        <v>5</v>
-      </c>
+      <c r="H18" s="7"/>
       <c r="I18" s="7" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24">
+        <v>20</v>
+      </c>
+      <c r="S18" s="7"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="7"/>
@@ -1913,36 +2415,40 @@
         <v>5</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24">
+        <v>1000</v>
+      </c>
+      <c r="S19" s="7"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D20" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>64</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="7"/>
@@ -1950,179 +2456,211 @@
         <v>5</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>17</v>
+        <v>129</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24">
+        <v>10</v>
+      </c>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24">
+        <v>100</v>
+      </c>
+      <c r="S20" s="7"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>66</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="5"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>67</v>
+        <v>129</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24">
+        <v>10</v>
+      </c>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24">
+        <v>100</v>
+      </c>
+      <c r="S21" s="7"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7">
         <v>6</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24">
+        <v>10</v>
+      </c>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24">
+        <v>200</v>
+      </c>
+      <c r="S22" s="7"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
+      <c r="H23" s="7">
+        <v>6</v>
+      </c>
       <c r="I23" s="7" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24">
+        <v>2</v>
+      </c>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24">
+        <v>20</v>
+      </c>
+      <c r="S23" s="7"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>26</v>
+        <v>15</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>68</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="7">
-        <v>7</v>
-      </c>
+      <c r="H24" s="7"/>
       <c r="I24" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24">
+        <v>20</v>
+      </c>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24">
+        <v>200</v>
+      </c>
+      <c r="S24" s="7"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -2131,51 +2669,104 @@
         <v>7</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24">
+        <v>20</v>
+      </c>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24">
+        <v>200</v>
+      </c>
+      <c r="S25" s="7"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="K26" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7">
+        <v>7</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24">
+        <v>1000</v>
+      </c>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24">
+        <v>2</v>
+      </c>
+      <c r="R26" s="24"/>
+      <c r="S26" s="7"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25">
+        <v>1000</v>
+      </c>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25">
+        <v>2</v>
+      </c>
+      <c r="R27" s="25"/>
+      <c r="S27" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2184,4 +2775,317 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE578F6-6E39-4770-8022-A43862711695}">
+  <dimension ref="B2:G75"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C25" s="20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C26" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C27" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C35" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="22"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C38" s="23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C40" s="21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C43" s="22"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C44" s="22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C45" s="22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C47" s="21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C48" s="22"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C57" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C58" s="22"/>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C59" s="23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C61" s="21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C64" s="22"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C65" s="22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C66" s="22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C68" s="21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C69" s="22"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C70" s="23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C73" s="22"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C74" s="22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C75" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>